<commit_message>
DESGLOCE DE COSTO SOCIAL
</commit_message>
<xml_diff>
--- a/NominasMaecco/bin/Debug/Archivos/tmmMaecco.xlsx
+++ b/NominasMaecco/bin/Debug/Archivos/tmmMaecco.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="85">
   <si>
     <t>TRABAJADOR</t>
   </si>
@@ -305,6 +305,18 @@
   </si>
   <si>
     <t>MAECCO JULIO 2018</t>
+  </si>
+  <si>
+    <t>IMSS_CS</t>
+  </si>
+  <si>
+    <t>RCV_CS</t>
+  </si>
+  <si>
+    <t>Infonavit_CS</t>
+  </si>
+  <si>
+    <t>ISN_CS</t>
   </si>
 </sst>
 </file>
@@ -729,7 +741,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -830,6 +842,7 @@
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1333,11 +1346,11 @@
   <sheetPr codeName="Hoja1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AE50"/>
+  <dimension ref="A1:AH50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="AI13" sqref="AI13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="14.25" x14ac:dyDescent="0.3"/>
@@ -1362,17 +1375,19 @@
     <col min="21" max="21" width="13.140625" style="39" customWidth="1"/>
     <col min="22" max="22" width="13.42578125" style="39" customWidth="1"/>
     <col min="23" max="23" width="15.5703125" style="39" customWidth="1"/>
-    <col min="24" max="24" width="3.42578125" style="39" customWidth="1"/>
-    <col min="25" max="25" width="17.5703125" style="39" customWidth="1"/>
-    <col min="26" max="26" width="17.28515625" style="39" customWidth="1"/>
-    <col min="27" max="27" width="15.28515625" style="39" customWidth="1"/>
-    <col min="28" max="28" width="18.7109375" style="39" customWidth="1"/>
-    <col min="29" max="29" width="11.5703125" style="39"/>
-    <col min="30" max="30" width="13.85546875" style="39" customWidth="1"/>
-    <col min="31" max="16384" width="11.5703125" style="39"/>
+    <col min="24" max="25" width="10.85546875" style="39" customWidth="1"/>
+    <col min="26" max="26" width="11.42578125" style="39" customWidth="1"/>
+    <col min="27" max="27" width="10.28515625" style="39" customWidth="1"/>
+    <col min="28" max="28" width="17.5703125" style="39" customWidth="1"/>
+    <col min="29" max="29" width="17.28515625" style="39" customWidth="1"/>
+    <col min="30" max="30" width="15.28515625" style="39" customWidth="1"/>
+    <col min="31" max="31" width="18.7109375" style="39" customWidth="1"/>
+    <col min="32" max="32" width="11.5703125" style="39"/>
+    <col min="33" max="33" width="13.85546875" style="39" customWidth="1"/>
+    <col min="34" max="16384" width="11.5703125" style="39"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" s="36" t="s">
         <v>14</v>
       </c>
@@ -1403,8 +1418,14 @@
       <c r="Z1" s="37"/>
       <c r="AA1" s="37"/>
       <c r="AB1" s="37"/>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AC1" s="37"/>
+      <c r="AD1" s="37"/>
+      <c r="AE1" s="37"/>
+      <c r="AF1" s="37"/>
+      <c r="AG1" s="37"/>
+      <c r="AH1" s="37"/>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" s="40"/>
       <c r="B2" s="40"/>
       <c r="C2" s="40"/>
@@ -1433,8 +1454,14 @@
       <c r="Z2" s="40"/>
       <c r="AA2" s="40"/>
       <c r="AB2" s="40"/>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AC2" s="40"/>
+      <c r="AD2" s="40"/>
+      <c r="AE2" s="40"/>
+      <c r="AF2" s="40"/>
+      <c r="AG2" s="40"/>
+      <c r="AH2" s="40"/>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" s="40"/>
       <c r="B3" s="40"/>
       <c r="C3" s="40"/>
@@ -1463,8 +1490,14 @@
       <c r="Z3" s="40"/>
       <c r="AA3" s="40"/>
       <c r="AB3" s="40"/>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AC3" s="40"/>
+      <c r="AD3" s="40"/>
+      <c r="AE3" s="40"/>
+      <c r="AF3" s="40"/>
+      <c r="AG3" s="40"/>
+      <c r="AH3" s="40"/>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" s="40"/>
       <c r="B4" s="40"/>
       <c r="C4" s="40"/>
@@ -1493,8 +1526,14 @@
       <c r="Z4" s="40"/>
       <c r="AA4" s="40"/>
       <c r="AB4" s="40"/>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AC4" s="40"/>
+      <c r="AD4" s="40"/>
+      <c r="AE4" s="40"/>
+      <c r="AF4" s="40"/>
+      <c r="AG4" s="40"/>
+      <c r="AH4" s="40"/>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" s="40"/>
       <c r="B5" s="40"/>
       <c r="C5" s="40"/>
@@ -1523,8 +1562,14 @@
       <c r="Z5" s="40"/>
       <c r="AA5" s="40"/>
       <c r="AB5" s="40"/>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AC5" s="40"/>
+      <c r="AD5" s="40"/>
+      <c r="AE5" s="40"/>
+      <c r="AF5" s="40"/>
+      <c r="AG5" s="40"/>
+      <c r="AH5" s="40"/>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" s="40"/>
       <c r="B6" s="40"/>
       <c r="C6" s="40"/>
@@ -1553,8 +1598,14 @@
       <c r="Z6" s="40"/>
       <c r="AA6" s="40"/>
       <c r="AB6" s="40"/>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AC6" s="40"/>
+      <c r="AD6" s="40"/>
+      <c r="AE6" s="40"/>
+      <c r="AF6" s="40"/>
+      <c r="AG6" s="40"/>
+      <c r="AH6" s="40"/>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" s="40"/>
       <c r="B7" s="40"/>
       <c r="C7" s="40"/>
@@ -1579,12 +1630,18 @@
       <c r="V7" s="40"/>
       <c r="W7" s="40"/>
       <c r="X7" s="40"/>
-      <c r="Y7" s="42"/>
+      <c r="Y7" s="40"/>
       <c r="Z7" s="40"/>
       <c r="AA7" s="40"/>
-      <c r="AB7" s="40"/>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AB7" s="42"/>
+      <c r="AC7" s="40"/>
+      <c r="AD7" s="40"/>
+      <c r="AE7" s="40"/>
+      <c r="AF7" s="40"/>
+      <c r="AG7" s="40"/>
+      <c r="AH7" s="40"/>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" s="43" t="s">
         <v>79</v>
       </c>
@@ -1615,136 +1672,154 @@
       <c r="Z8" s="40"/>
       <c r="AA8" s="40"/>
       <c r="AB8" s="40"/>
-    </row>
-    <row r="9" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="50" t="s">
+      <c r="AC8" s="40"/>
+      <c r="AD8" s="40"/>
+      <c r="AE8" s="40"/>
+      <c r="AF8" s="40"/>
+      <c r="AG8" s="40"/>
+      <c r="AH8" s="40"/>
+    </row>
+    <row r="9" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="50" t="s">
+      <c r="C9" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="50" t="s">
+      <c r="D9" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="50" t="s">
+      <c r="E9" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="50" t="s">
+      <c r="F9" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="50" t="s">
+      <c r="G9" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="H9" s="51" t="s">
+      <c r="H9" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="I9" s="50" t="s">
+      <c r="I9" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="J9" s="50" t="s">
+      <c r="J9" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="K9" s="50" t="s">
+      <c r="K9" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="L9" s="50" t="s">
+      <c r="L9" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="M9" s="50" t="s">
+      <c r="M9" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="N9" s="50" t="s">
+      <c r="N9" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="O9" s="51" t="s">
+      <c r="O9" s="52" t="s">
         <v>52</v>
       </c>
       <c r="P9" s="44"/>
-      <c r="Q9" s="50" t="s">
+      <c r="Q9" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="R9" s="50" t="s">
+      <c r="R9" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="S9" s="50" t="s">
+      <c r="S9" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="T9" s="50"/>
-      <c r="U9" s="50" t="s">
+      <c r="T9" s="51"/>
+      <c r="U9" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="V9" s="50" t="s">
+      <c r="V9" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="W9" s="50" t="s">
+      <c r="W9" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="X9" s="45"/>
-      <c r="Y9" s="50" t="s">
+      <c r="X9" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y9" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z9" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA9" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB9" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="Z9" s="46"/>
-      <c r="AA9" s="46"/>
-      <c r="AB9" s="50" t="s">
+      <c r="AC9" s="46"/>
+      <c r="AD9" s="46"/>
+      <c r="AE9" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="AD9" s="50" t="s">
+      <c r="AG9" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="AE9" s="50" t="s">
+      <c r="AH9" s="51" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="50"/>
-      <c r="B10" s="50"/>
-      <c r="C10" s="50"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="50"/>
-      <c r="J10" s="50"/>
-      <c r="K10" s="50"/>
-      <c r="L10" s="50"/>
-      <c r="M10" s="50"/>
-      <c r="N10" s="50"/>
-      <c r="O10" s="51"/>
+    <row r="10" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="51"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="51"/>
+      <c r="L10" s="51"/>
+      <c r="M10" s="51"/>
+      <c r="N10" s="51"/>
+      <c r="O10" s="52"/>
       <c r="P10" s="44"/>
-      <c r="Q10" s="50"/>
-      <c r="R10" s="50"/>
-      <c r="S10" s="50"/>
-      <c r="T10" s="50"/>
-      <c r="U10" s="50"/>
-      <c r="V10" s="50"/>
-      <c r="W10" s="50"/>
-      <c r="X10" s="45"/>
-      <c r="Y10" s="50"/>
-      <c r="Z10" s="45" t="s">
+      <c r="Q10" s="51"/>
+      <c r="R10" s="51"/>
+      <c r="S10" s="51"/>
+      <c r="T10" s="51"/>
+      <c r="U10" s="51"/>
+      <c r="V10" s="51"/>
+      <c r="W10" s="51"/>
+      <c r="X10" s="51"/>
+      <c r="Y10" s="51"/>
+      <c r="Z10" s="51"/>
+      <c r="AA10" s="51"/>
+      <c r="AB10" s="51"/>
+      <c r="AC10" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="AA10" s="45" t="s">
+      <c r="AD10" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="AB10" s="50"/>
-      <c r="AD10" s="50"/>
-      <c r="AE10" s="50"/>
-    </row>
-    <row r="11" spans="1:31" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="AB11" s="35" t="e">
-        <f>#REF!+#REF!+#REF!+#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:31" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:31" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:31" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:31" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:31" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+      <c r="AE10" s="51"/>
+      <c r="AG10" s="51"/>
+      <c r="AH10" s="51"/>
+    </row>
+    <row r="11" spans="1:34" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:34" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:34" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="AD13" s="50"/>
+      <c r="AE13" s="50"/>
+    </row>
+    <row r="14" spans="1:34" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:34" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:34" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="17" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="18" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="19" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -1784,8 +1859,7 @@
   <sortState ref="A11:AF23">
     <sortCondition ref="C11:C23"/>
   </sortState>
-  <mergeCells count="26">
-    <mergeCell ref="L9:L10"/>
+  <mergeCells count="30">
     <mergeCell ref="M9:M10"/>
     <mergeCell ref="N9:N10"/>
     <mergeCell ref="A9:A10"/>
@@ -1795,22 +1869,27 @@
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="G9:G10"/>
     <mergeCell ref="H9:H10"/>
-    <mergeCell ref="AD9:AD10"/>
-    <mergeCell ref="AE9:AE10"/>
+    <mergeCell ref="AH9:AH10"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="Q9:Q10"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="O9:O10"/>
     <mergeCell ref="J9:J10"/>
     <mergeCell ref="K9:K10"/>
+    <mergeCell ref="AE9:AE10"/>
+    <mergeCell ref="R9:R10"/>
     <mergeCell ref="AB9:AB10"/>
-    <mergeCell ref="R9:R10"/>
-    <mergeCell ref="Y9:Y10"/>
     <mergeCell ref="V9:V10"/>
     <mergeCell ref="U9:U10"/>
     <mergeCell ref="S9:S10"/>
     <mergeCell ref="T9:T10"/>
     <mergeCell ref="W9:W10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="X9:X10"/>
+    <mergeCell ref="Y9:Y10"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="AA9:AA10"/>
+    <mergeCell ref="AG9:AG10"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="28" orientation="landscape" r:id="rId1"/>
@@ -1863,39 +1942,39 @@
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
     </row>
     <row r="2" spans="1:39" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
     </row>
     <row r="3" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
       <c r="I3" s="8"/>
     </row>
     <row r="4" spans="1:39" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1972,15 +2051,15 @@
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="54"/>
       <c r="I7" s="8"/>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
@@ -2180,57 +2259,57 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="61"/>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="67" t="s">
+      <c r="C3" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="D3" s="67" t="s">
+      <c r="D3" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="67" t="s">
+      <c r="E3" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="67" t="s">
+      <c r="F3" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="61" t="s">
+      <c r="G3" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="H3" s="61" t="s">
+      <c r="H3" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="67" t="s">
+      <c r="I3" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="63" t="s">
+      <c r="J3" s="64" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="66"/>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="64"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="65"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="19"/>

</xml_diff>